<commit_message>
Emerson and life hist
Emerson SNP notes
Life hist workings
</commit_message>
<xml_diff>
--- a/lifehist/Vec Cap doodles.xlsx
+++ b/lifehist/Vec Cap doodles.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="10380" xr2:uid="{EA44F234-0235-4B0F-B02B-63910F787E96}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="10380" activeTab="1" xr2:uid="{EA44F234-0235-4B0F-B02B-63910F787E96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
   <si>
     <t>Vectorial capacity calculator</t>
   </si>
@@ -413,26 +414,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BC3E3E-6BA4-40A9-8249-F22A2F19FFBA}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -440,7 +441,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -469,7 +470,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -498,7 +499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -527,7 +528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -556,7 +557,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D9">
         <f>((D5*D6^2)*D8)*D7</f>
         <v>40000</v>
@@ -590,4 +591,196 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0208558E-EA25-46F2-961A-57E887AEE780}">
+  <dimension ref="B2:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="27.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1E-3</v>
+      </c>
+      <c r="E3">
+        <v>1E-3</v>
+      </c>
+      <c r="F3">
+        <v>1E-3</v>
+      </c>
+      <c r="G3">
+        <v>1E-3</v>
+      </c>
+      <c r="H3">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>3000</v>
+      </c>
+      <c r="F4">
+        <v>3000</v>
+      </c>
+      <c r="G4">
+        <v>3000</v>
+      </c>
+      <c r="H4">
+        <v>1000</v>
+      </c>
+      <c r="I4">
+        <v>3000</v>
+      </c>
+      <c r="J4">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
+      <c r="H7">
+        <v>0.3</v>
+      </c>
+      <c r="I7">
+        <v>0.2</v>
+      </c>
+      <c r="J7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="D8">
+        <f>((D4*D5^2)*D7)*D6*D3</f>
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:H8" si="0">((E4*E5^2)*E7)*E6*E3</f>
+        <v>120</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ref="E8:J8" si="1">((I4*I5^2)*I7)*I6</f>
+        <v>48000</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>16200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>